<commit_message>
discovered error in writing to original sample file.  Will fix tonight.
</commit_message>
<xml_diff>
--- a/sant_csv.xlsx
+++ b/sant_csv.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blake\workspace\Excel-to-PDF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blake\workspace\Excel-to-PDF\excel-to-pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6587"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -59,64 +59,22 @@
     <t>You're truly in the stars.&amp;&amp;LRest in piece.</t>
   </si>
   <si>
-    <t>First Last</t>
-  </si>
-  <si>
-    <t>AAA-BB-1234</t>
-  </si>
-  <si>
-    <t>11 12 13.4, 55 66 77.8</t>
-  </si>
-  <si>
-    <t>bbopper321@hotmail.com</t>
-  </si>
-  <si>
     <t>Brightness</t>
   </si>
   <si>
     <t>Extra Bright</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>tinyurl</t>
   </si>
   <si>
     <t>sample url 1</t>
   </si>
   <si>
-    <t>sample url 2</t>
-  </si>
-  <si>
     <t>Binary?</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>KyleSant</t>
-  </si>
-  <si>
-    <t>ZZZ-ZZ-9999</t>
-  </si>
-  <si>
-    <t>12 34 56.7, 89 01 23.4</t>
-  </si>
-  <si>
-    <t>Sample message</t>
-  </si>
-  <si>
-    <t>bd21@uw.edu</t>
-  </si>
-  <si>
-    <t>Bright</t>
-  </si>
-  <si>
-    <t>sample url 3</t>
   </si>
 </sst>
 </file>
@@ -485,21 +443,21 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A4" sqref="A3:X4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.59765625" customWidth="1"/>
-    <col min="7" max="7" width="31.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.17578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.64453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.64453125" customWidth="1"/>
+    <col min="5" max="5" width="18.5859375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5859375" customWidth="1"/>
+    <col min="7" max="7" width="31.1171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1171875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +468,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -522,13 +480,13 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -539,7 +497,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -551,74 +509,25 @@
         <v>8</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1">
-        <v>42726</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>20</v>
-      </c>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B3" s="1"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="1">
-        <v>42732</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>30</v>
-      </c>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B4" s="1"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the actual csv input file.  got the text replacement working by making copies and then replacing.
</commit_message>
<xml_diff>
--- a/sant_csv.xlsx
+++ b/sant_csv.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blake\workspace\Excel-to-PDF\excel-to-pdf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blake\workspace\Excel-to-PDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6587"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6583"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -75,6 +75,27 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>First Last</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>ABC-DE-1234</t>
+  </si>
+  <si>
+    <t>message 1.  message 2.</t>
+  </si>
+  <si>
+    <t>asdf@gmail.com</t>
+  </si>
+  <si>
+    <t>Bright</t>
+  </si>
+  <si>
+    <t>url2</t>
   </si>
 </sst>
 </file>
@@ -119,12 +140,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -440,24 +462,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A3:X4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.17578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.64453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.64453125" customWidth="1"/>
-    <col min="5" max="5" width="18.5859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5859375" customWidth="1"/>
-    <col min="7" max="7" width="31.1171875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.1171875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.61328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.61328125" customWidth="1"/>
+    <col min="5" max="5" width="18.61328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.07421875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.07421875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,20 +494,20 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H1" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -502,32 +523,58 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H2" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B3" s="1"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4029</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
-      <c r="H4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>